<commit_message>
Added grouped backend values.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\WORKDIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B84FA5F-0FB2-4430-A383-1628319E426E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45EB5C6-9B94-4E78-A614-D248140E1A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
+    <workbookView xWindow="-28920" yWindow="-3285" windowWidth="29040" windowHeight="15840" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
   </bookViews>
   <sheets>
     <sheet name="machine_readable" sheetId="7" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="231">
   <si>
     <t>INPUTS</t>
   </si>
@@ -685,19 +685,52 @@
     <t>2028-2029</t>
   </si>
   <si>
-    <t>annual_public_debt_charges</t>
-  </si>
-  <si>
     <t>outputs</t>
   </si>
   <si>
     <t>Frais annuels de la dette publique</t>
   </si>
   <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>Résultats</t>
+    <t>Cumulative surplus/(deficit)</t>
+  </si>
+  <si>
+    <t>Surplus/(déficit) cumulatif</t>
+  </si>
+  <si>
+    <t>is_static</t>
+  </si>
+  <si>
+    <t>Surplus/(déficit) pour l'année</t>
+  </si>
+  <si>
+    <t>Inclut le service de la dette publique sur le surplus/(déficit) des années précédentes résultant des politiques mises en œuvre.</t>
+  </si>
+  <si>
+    <t>Includes public debt charges on surplus/(deficit) from previous years resulting from the implemented policies.</t>
+  </si>
+  <si>
+    <t>Frais cumulatifs de la dette publique</t>
+  </si>
+  <si>
+    <t>backend</t>
+  </si>
+  <si>
+    <t>Taux des bons du Trésor à 90 jours</t>
+  </si>
+  <si>
+    <t>Taux d'intérêt</t>
+  </si>
+  <si>
+    <t>Interest rates</t>
+  </si>
+  <si>
+    <t>Long-term bonds rate</t>
+  </si>
+  <si>
+    <t>Surplus for the year</t>
+  </si>
+  <si>
+    <t>Taux des obligations à long terme</t>
   </si>
 </sst>
 </file>
@@ -1364,15 +1397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DA5658-E2EA-4E0B-B547-2D4F388F10E4}">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" style="21" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" style="21" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
@@ -1380,10 +1414,10 @@
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="11" width="25.7109375" customWidth="1"/>
+    <col min="10" max="12" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>205</v>
       </c>
@@ -1415,25 +1449,28 @@
         <v>201</v>
       </c>
       <c r="K1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" t="s">
         <v>207</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>202</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>203</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>204</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>213</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>209</v>
       </c>
@@ -1452,14 +1489,12 @@
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
       <c r="M2">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1470,8 +1505,11 @@
       <c r="P2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -1490,12 +1528,10 @@
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="15"/>
+      <c r="L3" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
       <c r="M3">
         <v>0</v>
       </c>
@@ -1508,58 +1544,67 @@
       <c r="P3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>215</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>216</v>
       </c>
       <c r="C4" s="73" t="s">
         <v>67</v>
       </c>
       <c r="D4" s="73" t="s">
-        <v>217</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>219</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="15"/>
+      <c r="L4" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f>'For user (EN)'!C10</f>
-        <v>0</v>
-      </c>
-      <c r="M4">
+        <v>36.021489692499657</v>
+      </c>
+      <c r="N4">
         <f>'For user (EN)'!D10</f>
-        <v>0</v>
-      </c>
-      <c r="N4">
+        <v>37.319037412166516</v>
+      </c>
+      <c r="O4">
         <f>'For user (EN)'!E10</f>
-        <v>0</v>
-      </c>
-      <c r="O4">
+        <v>29.208615938255132</v>
+      </c>
+      <c r="P4">
         <f>'For user (EN)'!F10</f>
-        <v>0</v>
-      </c>
-      <c r="P4">
+        <v>30.003464565959376</v>
+      </c>
+      <c r="Q4">
         <f>'For user (EN)'!G10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
+        <v>30.819943261390854</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>218</v>
+      </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -1567,23 +1612,91 @@
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
+      <c r="L5" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="M5">
+        <f>'For user (EN)'!C11</f>
+        <v>1036.0214896924997</v>
+      </c>
+      <c r="N5">
+        <f>'For user (EN)'!D11</f>
+        <v>1073.3405271046663</v>
+      </c>
+      <c r="O5">
+        <f>'For user (EN)'!E11</f>
+        <v>1102.5491430429215</v>
+      </c>
+      <c r="P5">
+        <f>'For user (EN)'!F11</f>
+        <v>1132.5526076088809</v>
+      </c>
+      <c r="Q5">
+        <f>'For user (EN)'!G11</f>
+        <v>1163.3725508702717</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>220</v>
+      </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="I6" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>221</v>
+      </c>
       <c r="K6" s="15"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
+      <c r="L6" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="M6">
+        <f>'For user (EN)'!C12</f>
+        <v>1036.0214896924997</v>
+      </c>
+      <c r="N6">
+        <f>'For user (EN)'!D12</f>
+        <v>37.319037412166516</v>
+      </c>
+      <c r="O6">
+        <f>'For user (EN)'!E12</f>
+        <v>29.208615938255132</v>
+      </c>
+      <c r="P6">
+        <f>'For user (EN)'!F12</f>
+        <v>30.003464565959376</v>
+      </c>
+      <c r="Q6">
+        <f>'For user (EN)'!G12</f>
+        <v>30.819943261390854</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>223</v>
+      </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -1591,32 +1704,127 @@
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="L7" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="M7">
+        <f>'For user (EN)'!C13</f>
+        <v>36.021489692499657</v>
+      </c>
+      <c r="N7">
+        <f>'For user (EN)'!D13</f>
+        <v>73.340527104666165</v>
+      </c>
+      <c r="O7">
+        <f>'For user (EN)'!E13</f>
+        <v>102.5491430429213</v>
+      </c>
+      <c r="P7">
+        <f>'For user (EN)'!F13</f>
+        <v>132.55260760888069</v>
+      </c>
+      <c r="Q7">
+        <f>'For user (EN)'!G13</f>
+        <v>163.37255087027154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="73" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>226</v>
+      </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="K8" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="24">
+        <f>Model!D10</f>
+        <v>3.7</v>
+      </c>
+      <c r="N8" s="24">
+        <f>Model!E10</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="O8" s="24">
+        <f>Model!F10</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="P8" s="24">
+        <f>Model!G10</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="Q8" s="24">
+        <f>Model!H10</f>
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>228</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>226</v>
+      </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K9" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="15"/>
+      <c r="M9" s="24">
+        <f>Model!D11</f>
+        <v>3.5207104999999999</v>
+      </c>
+      <c r="N9" s="24">
+        <f>Model!E11</f>
+        <v>3.5</v>
+      </c>
+      <c r="O9" s="24">
+        <f>Model!F11</f>
+        <v>3.5</v>
+      </c>
+      <c r="P9" s="24">
+        <f>Model!G11</f>
+        <v>3.5</v>
+      </c>
+      <c r="Q9" s="24">
+        <f>Model!H11</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="73"/>
       <c r="D10" s="73"/>
@@ -1627,8 +1835,9 @@
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="C11" s="73"/>
       <c r="D11" s="73"/>
@@ -1639,8 +1848,9 @@
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" s="73"/>
       <c r="D12" s="73"/>
@@ -1651,8 +1861,9 @@
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
       <c r="C13" s="73"/>
       <c r="D13" s="73"/>
@@ -1663,8 +1874,9 @@
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
       <c r="C14" s="73"/>
       <c r="D14" s="73"/>
@@ -1675,8 +1887,9 @@
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="73"/>
       <c r="D15" s="73"/>
@@ -1687,8 +1900,9 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" s="73"/>
       <c r="D16" s="73"/>
@@ -1699,8 +1913,9 @@
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" s="73"/>
       <c r="D17" s="73"/>
@@ -1711,8 +1926,9 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" s="73"/>
       <c r="D18" s="73"/>
@@ -1723,8 +1939,9 @@
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" s="73"/>
       <c r="D19" s="73"/>
@@ -1735,8 +1952,9 @@
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="15"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="73"/>
       <c r="D20" s="73"/>
@@ -1747,8 +1965,9 @@
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" s="73"/>
       <c r="D21" s="73"/>
@@ -1759,8 +1978,9 @@
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" s="73"/>
       <c r="D22" s="73"/>
@@ -1771,8 +1991,9 @@
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="15"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" s="73"/>
       <c r="D23" s="73"/>
@@ -1783,8 +2004,9 @@
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="15"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" s="73"/>
       <c r="D24" s="73"/>
@@ -1795,8 +2017,9 @@
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="15"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="15"/>
       <c r="C25" s="73"/>
       <c r="D25" s="73"/>
@@ -1807,8 +2030,9 @@
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="15"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="73"/>
       <c r="D26" s="73"/>
@@ -1819,8 +2043,9 @@
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="15"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="73"/>
       <c r="D27" s="73"/>
@@ -1831,8 +2056,9 @@
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="15"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="15"/>
       <c r="C28" s="73"/>
       <c r="D28" s="73"/>
@@ -1843,8 +2069,9 @@
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="15"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="73"/>
       <c r="D29" s="73"/>
@@ -1855,8 +2082,9 @@
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="15"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="C30" s="73"/>
       <c r="D30" s="73"/>
@@ -1867,8 +2095,9 @@
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="15"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="15"/>
       <c r="C31" s="73"/>
       <c r="D31" s="73"/>
@@ -1879,8 +2108,9 @@
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="15"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
       <c r="C32" s="73"/>
       <c r="D32" s="73"/>
@@ -1891,8 +2121,9 @@
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="15"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="15"/>
       <c r="C33" s="73"/>
       <c r="D33" s="73"/>
@@ -1903,8 +2134,9 @@
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="15"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="15"/>
       <c r="C34" s="73"/>
       <c r="D34" s="73"/>
@@ -1915,8 +2147,9 @@
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="15"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="15"/>
       <c r="C35" s="73"/>
       <c r="D35" s="73"/>
@@ -1927,8 +2160,9 @@
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="15"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="15"/>
       <c r="C36" s="73"/>
       <c r="D36" s="73"/>
@@ -1939,6 +2173,7 @@
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1954,7 +2189,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,23 +2262,23 @@
         <v>5</v>
       </c>
       <c r="C4" s="4">
-        <f>machine_readable!L2</f>
-        <v>0</v>
+        <f>machine_readable!M2</f>
+        <v>1000</v>
       </c>
       <c r="D4" s="4">
-        <f>machine_readable!M2</f>
+        <f>machine_readable!N2</f>
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <f>machine_readable!N2</f>
+        <f>machine_readable!O2</f>
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <f>machine_readable!O2</f>
+        <f>machine_readable!P2</f>
         <v>0</v>
       </c>
       <c r="G4" s="4">
-        <f>machine_readable!P2</f>
+        <f>machine_readable!Q2</f>
         <v>0</v>
       </c>
     </row>
@@ -2055,23 +2290,23 @@
         <v>5</v>
       </c>
       <c r="C5" s="4">
-        <f>machine_readable!L3</f>
+        <f>machine_readable!M3</f>
         <v>0</v>
       </c>
       <c r="D5" s="4">
-        <f>machine_readable!M3</f>
+        <f>machine_readable!N3</f>
         <v>0</v>
       </c>
       <c r="E5" s="4">
-        <f>machine_readable!N3</f>
+        <f>machine_readable!O3</f>
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <f>machine_readable!O3</f>
+        <f>machine_readable!P3</f>
         <v>0</v>
       </c>
       <c r="G5" s="4">
-        <f>machine_readable!P3</f>
+        <f>machine_readable!Q3</f>
         <v>0</v>
       </c>
     </row>
@@ -2084,7 +2319,7 @@
       </c>
       <c r="C6" s="68">
         <f t="shared" ref="C6:G6" si="2">C4-C5</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="68">
         <f t="shared" si="2"/>
@@ -2123,23 +2358,23 @@
       </c>
       <c r="C10" s="13">
         <f>Model!D53</f>
-        <v>0</v>
+        <v>36.021489692499657</v>
       </c>
       <c r="D10" s="13">
         <f>Model!E53</f>
-        <v>0</v>
+        <v>37.319037412166516</v>
       </c>
       <c r="E10" s="13">
         <f>Model!F53</f>
-        <v>0</v>
+        <v>29.208615938255132</v>
       </c>
       <c r="F10" s="13">
         <f>Model!G53</f>
-        <v>0</v>
+        <v>30.003464565959376</v>
       </c>
       <c r="G10" s="13">
         <f>Model!H53</f>
-        <v>0</v>
+        <v>30.819943261390854</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2151,23 +2386,23 @@
       </c>
       <c r="C11" s="13">
         <f>Model!D54</f>
-        <v>0</v>
+        <v>1036.0214896924997</v>
       </c>
       <c r="D11" s="13">
         <f>Model!E54</f>
-        <v>0</v>
+        <v>1073.3405271046663</v>
       </c>
       <c r="E11" s="13">
         <f>Model!F54</f>
-        <v>0</v>
+        <v>1102.5491430429215</v>
       </c>
       <c r="F11" s="13">
         <f>Model!G54</f>
-        <v>0</v>
+        <v>1132.5526076088809</v>
       </c>
       <c r="G11" s="13">
         <f>Model!H54</f>
-        <v>0</v>
+        <v>1163.3725508702717</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2179,23 +2414,23 @@
       </c>
       <c r="C12" s="13">
         <f>Model!D53+Model!D6</f>
-        <v>0</v>
+        <v>1036.0214896924997</v>
       </c>
       <c r="D12" s="13">
         <f>Model!E53+Model!E6</f>
-        <v>0</v>
+        <v>37.319037412166516</v>
       </c>
       <c r="E12" s="13">
         <f>Model!F53+Model!F6</f>
-        <v>0</v>
+        <v>29.208615938255132</v>
       </c>
       <c r="F12" s="13">
         <f>Model!G53+Model!G6</f>
-        <v>0</v>
+        <v>30.003464565959376</v>
       </c>
       <c r="G12" s="13">
         <f>Model!H53+Model!H6</f>
-        <v>0</v>
+        <v>30.819943261390854</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2207,23 +2442,23 @@
       </c>
       <c r="C13" s="51">
         <f>SUM($C10:C10)</f>
-        <v>0</v>
+        <v>36.021489692499657</v>
       </c>
       <c r="D13" s="51">
         <f>SUM($C10:D10)</f>
-        <v>0</v>
+        <v>73.340527104666165</v>
       </c>
       <c r="E13" s="51">
         <f>SUM($C10:E10)</f>
-        <v>0</v>
+        <v>102.5491430429213</v>
       </c>
       <c r="F13" s="51">
         <f>SUM($C10:F10)</f>
-        <v>0</v>
+        <v>132.55260760888069</v>
       </c>
       <c r="G13" s="51">
         <f>SUM($C10:G10)</f>
-        <v>0</v>
+        <v>163.37255087027154</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2253,8 +2488,8 @@
   </sheetPr>
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,7 +2570,7 @@
       </c>
       <c r="D4" s="4">
         <f>'For user (EN)'!C4</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E4" s="4">
         <f>'For user (EN)'!D4</f>
@@ -2393,7 +2628,7 @@
       </c>
       <c r="D6" s="68">
         <f>'For user (EN)'!C6</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E6" s="68">
         <f>'For user (EN)'!D6</f>
@@ -2584,7 +2819,7 @@
       <c r="C16" s="30"/>
       <c r="D16" s="9">
         <f>(D13/100)*D6</f>
-        <v>0</v>
+        <v>36.021489692499657</v>
       </c>
       <c r="E16" s="9">
         <f>(E13/100)*E6</f>
@@ -2617,19 +2852,19 @@
       </c>
       <c r="E17" s="9">
         <f>(D50/100)*D54</f>
-        <v>0</v>
+        <v>37.319037412166516</v>
       </c>
       <c r="F17" s="9">
         <f>(E50/100)*E54</f>
-        <v>0</v>
+        <v>29.208615938255132</v>
       </c>
       <c r="G17" s="9">
         <f>(F50/100)*F54</f>
-        <v>0</v>
+        <v>30.003464565959376</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" ref="H17" si="2">(G50/100)*G54</f>
-        <v>0</v>
+        <v>30.819943261390854</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -2642,23 +2877,23 @@
       <c r="C18" s="30"/>
       <c r="D18" s="9">
         <f>-(D6+D16+D17)</f>
-        <v>0</v>
+        <v>-1036.0214896924997</v>
       </c>
       <c r="E18" s="9">
         <f>-(E6+E16+E17)</f>
-        <v>0</v>
+        <v>-37.319037412166516</v>
       </c>
       <c r="F18" s="9">
         <f>-(F6+F16+F17)</f>
-        <v>0</v>
+        <v>-29.208615938255132</v>
       </c>
       <c r="G18" s="9">
         <f>-(G6+G16+G17)</f>
-        <v>0</v>
+        <v>-30.003464565959376</v>
       </c>
       <c r="H18" s="9">
         <f t="shared" ref="H18" si="3">-(H6+H16+H17)</f>
-        <v>0</v>
+        <v>-30.819943261390854</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2671,23 +2906,23 @@
       <c r="C19" s="30"/>
       <c r="D19" s="9">
         <f>SUM($D18:D18)</f>
-        <v>0</v>
+        <v>-1036.0214896924997</v>
       </c>
       <c r="E19" s="9">
         <f>SUM($D18:E18)</f>
-        <v>0</v>
+        <v>-1073.3405271046663</v>
       </c>
       <c r="F19" s="9">
         <f>SUM($D18:F18)</f>
-        <v>0</v>
+        <v>-1102.5491430429215</v>
       </c>
       <c r="G19" s="9">
         <f>SUM($D18:G18)</f>
-        <v>0</v>
+        <v>-1132.5526076088809</v>
       </c>
       <c r="H19" s="9">
         <f>SUM($D18:H18)</f>
-        <v>0</v>
+        <v>-1163.3725508702717</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2722,23 +2957,23 @@
       <c r="C22" s="30"/>
       <c r="D22" s="9">
         <f>SUM(D18,D35,D39)*'Fiscal Model Import'!E2</f>
-        <v>0</v>
+        <v>-576.1076583314034</v>
       </c>
       <c r="E22" s="9">
         <f>SUM(E18,E35,E39)*'Fiscal Model Import'!F2</f>
-        <v>0</v>
+        <v>-20.752256076354762</v>
       </c>
       <c r="F22" s="9">
         <f>SUM(F18,F35,F39)*'Fiscal Model Import'!G2</f>
-        <v>0</v>
+        <v>-16.242237732234653</v>
       </c>
       <c r="G22" s="9">
         <f>SUM(G18,G35,G39)*'Fiscal Model Import'!H2</f>
-        <v>0</v>
+        <v>-16.684234723793711</v>
       </c>
       <c r="H22" s="9">
         <f>SUM(H18,H35,H39)*'Fiscal Model Import'!I2</f>
-        <v>0</v>
+        <v>-17.138259697196649</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -2751,23 +2986,23 @@
       <c r="C23" s="30"/>
       <c r="D23" s="69">
         <f>SUM(D18,D35,D39)*'Fiscal Model Import'!E4</f>
-        <v>0</v>
+        <v>-354.13365014804413</v>
       </c>
       <c r="E23" s="69">
         <f>SUM(E18,E35,E39)*'Fiscal Model Import'!F4</f>
-        <v>0</v>
+        <v>-12.756421628575051</v>
       </c>
       <c r="F23" s="69">
         <f>SUM(F18,F35,F39)*'Fiscal Model Import'!G4</f>
-        <v>0</v>
+        <v>-9.9841112186357694</v>
       </c>
       <c r="G23" s="69">
         <f>SUM(G18,G35,G39)*'Fiscal Model Import'!H4</f>
-        <v>0</v>
+        <v>-10.255806978467561</v>
       </c>
       <c r="H23" s="69">
         <f>SUM(H18,H35,H39)*'Fiscal Model Import'!I4</f>
-        <v>0</v>
+        <v>-10.534896344429537</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -2780,23 +3015,23 @@
       <c r="C24" s="30"/>
       <c r="D24" s="69">
         <f>SUM(D18,D35,D39)*'Fiscal Model Import'!E3</f>
-        <v>0</v>
+        <v>-105.78018121305216</v>
       </c>
       <c r="E24" s="69">
         <f>SUM(E18,E35,E39)*'Fiscal Model Import'!F3</f>
-        <v>0</v>
+        <v>-3.8103597072367039</v>
       </c>
       <c r="F24" s="69">
         <f>SUM(F18,F35,F39)*'Fiscal Model Import'!G3</f>
-        <v>0</v>
+        <v>-2.982266987384711</v>
       </c>
       <c r="G24" s="69">
         <f>SUM(G18,G35,G39)*'Fiscal Model Import'!H3</f>
-        <v>0</v>
+        <v>-3.0634228636981029</v>
       </c>
       <c r="H24" s="69">
         <f>SUM(H18,H35,H39)*'Fiscal Model Import'!I3</f>
-        <v>0</v>
+        <v>-3.1467872197646676</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2867,23 +3102,23 @@
       <c r="C27" s="30"/>
       <c r="D27" s="9">
         <f>D22</f>
-        <v>0</v>
+        <v>-576.1076583314034</v>
       </c>
       <c r="E27" s="69">
         <f>IF(AND(SUM(E$18,E$35,E$39)&gt;0,E19&gt;0),D27+E22-E35,E$19*D30)</f>
-        <v>0</v>
+        <v>-596.8599144077582</v>
       </c>
       <c r="F27" s="69">
         <f>IF(AND(SUM(F$18,F$35,F$39)&gt;0,F19&gt;0),E27+F22-F35,F$19*E30)</f>
-        <v>0</v>
+        <v>-613.10215213999288</v>
       </c>
       <c r="G27" s="69">
         <f t="shared" ref="G27:H27" si="4">IF(AND(SUM(G$18,G$35,G$39)&gt;0,G19&gt;0),F27+G22-G35,G$19*F30)</f>
-        <v>0</v>
+        <v>-629.78638686378656</v>
       </c>
       <c r="H27" s="69">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-646.92464656098321</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -2896,23 +3131,23 @@
       <c r="C28" s="30"/>
       <c r="D28" s="69">
         <f>D23</f>
-        <v>0</v>
+        <v>-354.13365014804413</v>
       </c>
       <c r="E28" s="69">
         <f>IF(AND(SUM(E$18,E$35,E$39)&gt;0,E19&gt;0),D28+E23-E39,E$19*D31)</f>
-        <v>0</v>
+        <v>-366.89007177661921</v>
       </c>
       <c r="F28" s="69">
         <f t="shared" ref="F28:H28" si="5">IF(AND(SUM(F$18,F$35,F$39)&gt;0,F19&gt;0),E28+F23-F39,F$19*E31)</f>
-        <v>0</v>
+        <v>-376.87418299525501</v>
       </c>
       <c r="G28" s="69">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-387.12998997372256</v>
       </c>
       <c r="H28" s="69">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-397.66488631815207</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -2925,23 +3160,23 @@
       <c r="C29" s="30"/>
       <c r="D29" s="69">
         <f>D24</f>
-        <v>0</v>
+        <v>-105.78018121305216</v>
       </c>
       <c r="E29" s="69">
         <f>IF(AND(SUM(E$18,E$35,E$39)&gt;0,E19&gt;0),D29+E24,E$19*D32)</f>
-        <v>0</v>
+        <v>-109.59054092028887</v>
       </c>
       <c r="F29" s="69">
         <f t="shared" ref="F29:H29" si="6">IF(AND(SUM(F$18,F$35,F$39)&gt;0,F19&gt;0),E29+F24,F$19*E32)</f>
-        <v>0</v>
+        <v>-112.57280790767358</v>
       </c>
       <c r="G29" s="69">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-115.63623077137169</v>
       </c>
       <c r="H29" s="69">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-118.78301799113635</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2954,23 +3189,23 @@
       <c r="C30" s="30"/>
       <c r="D30" s="67">
         <f>IF(D19=0,0,D27/D19)</f>
-        <v>0</v>
+        <v>0.55607693861871266</v>
       </c>
       <c r="E30" s="67">
         <f t="shared" ref="E30:H30" si="7">IF(E19=0,0,E27/E19)</f>
-        <v>0</v>
+        <v>0.55607693861871266</v>
       </c>
       <c r="F30" s="67">
         <f>IF(F19=0,0,F27/F19)</f>
-        <v>0</v>
+        <v>0.55607693861871266</v>
       </c>
       <c r="G30" s="67">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.55607693861871266</v>
       </c>
       <c r="H30" s="67">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.55607693861871266</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2983,23 +3218,23 @@
       <c r="C31" s="30"/>
       <c r="D31" s="67">
         <f>IF(D19=0,0,D28/D19)</f>
-        <v>0</v>
+        <v>0.34182075726359124</v>
       </c>
       <c r="E31" s="67">
         <f t="shared" ref="E31:H31" si="8">IF(E19=0,0,E28/E19)</f>
-        <v>0</v>
+        <v>0.34182075726359124</v>
       </c>
       <c r="F31" s="67">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.34182075726359124</v>
       </c>
       <c r="G31" s="67">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.34182075726359124</v>
       </c>
       <c r="H31" s="67">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.34182075726359124</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3012,23 +3247,23 @@
       <c r="C32" s="30"/>
       <c r="D32" s="67">
         <f>IF(D19=0,0,D29/D19)</f>
-        <v>0</v>
+        <v>0.10210230411769609</v>
       </c>
       <c r="E32" s="67">
         <f t="shared" ref="E32:H32" si="9">IF(E19=0,0,E29/E19)</f>
-        <v>0</v>
+        <v>0.10210230411769609</v>
       </c>
       <c r="F32" s="67">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.10210230411769609</v>
       </c>
       <c r="G32" s="67">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.10210230411769609</v>
       </c>
       <c r="H32" s="67">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.10210230411769609</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3205,7 +3440,7 @@
       <c r="D42" s="46"/>
       <c r="E42" s="32">
         <f>IF(D19&lt;0,E12,D12)</f>
-        <v>3.4672898500000002</v>
+        <v>2.93</v>
       </c>
       <c r="F42" s="32">
         <f>IF(OR(E19&lt;0,(E28-F39)=0),F12,(E47*E28-F41*F39)/(E28-F39))</f>
@@ -3420,23 +3655,23 @@
       <c r="C53" s="12"/>
       <c r="D53" s="13">
         <f>D16+D17</f>
-        <v>0</v>
+        <v>36.021489692499657</v>
       </c>
       <c r="E53" s="13">
         <f>E16+E17</f>
-        <v>0</v>
+        <v>37.319037412166516</v>
       </c>
       <c r="F53" s="13">
         <f>F16+F17</f>
-        <v>0</v>
+        <v>29.208615938255132</v>
       </c>
       <c r="G53" s="13">
         <f t="shared" ref="G53:H53" si="18">G16+G17</f>
-        <v>0</v>
+        <v>30.003464565959376</v>
       </c>
       <c r="H53" s="13">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>30.819943261390854</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3447,23 +3682,23 @@
       <c r="C54" s="12"/>
       <c r="D54" s="13">
         <f t="shared" ref="D54:H54" si="19">-D19</f>
-        <v>0</v>
+        <v>1036.0214896924997</v>
       </c>
       <c r="E54" s="13">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1073.3405271046663</v>
       </c>
       <c r="F54" s="13">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1102.5491430429215</v>
       </c>
       <c r="G54" s="13">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1132.5526076088809</v>
       </c>
       <c r="H54" s="13">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1163.3725508702717</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3474,23 +3709,23 @@
       <c r="C55" s="12"/>
       <c r="D55" s="13">
         <f>SUM($D53:D53)</f>
-        <v>0</v>
+        <v>36.021489692499657</v>
       </c>
       <c r="E55" s="13">
         <f>SUM($D53:E53)</f>
-        <v>0</v>
+        <v>73.340527104666165</v>
       </c>
       <c r="F55" s="13">
         <f>SUM($D53:F53)</f>
-        <v>0</v>
+        <v>102.5491430429213</v>
       </c>
       <c r="G55" s="13">
         <f>SUM($D53:G53)</f>
-        <v>0</v>
+        <v>132.55260760888069</v>
       </c>
       <c r="H55" s="13">
         <f>SUM($D53:H53)</f>
-        <v>0</v>
+        <v>163.37255087027154</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Allow for empty fiscal years.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\WORKDIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45EB5C6-9B94-4E78-A614-D248140E1A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF752891-D999-47CC-8055-575D0199C694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3285" windowWidth="29040" windowHeight="15840" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
+    <workbookView xWindow="-57720" yWindow="-3285" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
   </bookViews>
   <sheets>
-    <sheet name="machine_readable" sheetId="7" r:id="rId1"/>
-    <sheet name="For user (EN)" sheetId="2" r:id="rId2"/>
-    <sheet name="Model" sheetId="1" r:id="rId3"/>
-    <sheet name="Fiscal Model Import" sheetId="5" r:id="rId4"/>
-    <sheet name="Decomposition" sheetId="6" r:id="rId5"/>
+    <sheet name="How to interface with Web tool" sheetId="8" r:id="rId1"/>
+    <sheet name="machine_readable" sheetId="7" r:id="rId2"/>
+    <sheet name="For user (EN)" sheetId="2" r:id="rId3"/>
+    <sheet name="Model" sheetId="1" r:id="rId4"/>
+    <sheet name="Fiscal Model Import" sheetId="5" r:id="rId5"/>
+    <sheet name="Decomposition" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="290">
   <si>
     <t>INPUTS</t>
   </si>
@@ -731,6 +732,183 @@
   </si>
   <si>
     <t>Taux des obligations à long terme</t>
+  </si>
+  <si>
+    <t>Taux des obligations à moyen terme</t>
+  </si>
+  <si>
+    <t>Medium-term bonds rate</t>
+  </si>
+  <si>
+    <t>Marginal effective interest rate</t>
+  </si>
+  <si>
+    <t>Taux d'intérêt marginal effectif</t>
+  </si>
+  <si>
+    <t>Frais de la dette sur les soldes primaires</t>
+  </si>
+  <si>
+    <t>Nouvelle dette globale</t>
+  </si>
+  <si>
+    <t>Overall new debt</t>
+  </si>
+  <si>
+    <t>Charges de la dette sur le stock de la dette existante</t>
+  </si>
+  <si>
+    <t>Nouveau besoin d'emprunt</t>
+  </si>
+  <si>
+    <t>Encours de la dette</t>
+  </si>
+  <si>
+    <t>Bons du Trésor : émission</t>
+  </si>
+  <si>
+    <t>Government Bonds Composition (Issuance &amp; Stock)</t>
+  </si>
+  <si>
+    <t>Obligations gouvernementales Composition (émission et stock)</t>
+  </si>
+  <si>
+    <t>Obligations à moyen terme : émission</t>
+  </si>
+  <si>
+    <t>Obligations à long terme : émission</t>
+  </si>
+  <si>
+    <t>Obligations à moyen terme : emprunts cumulés</t>
+  </si>
+  <si>
+    <t>Obligations à long terme : emprunts cumulés</t>
+  </si>
+  <si>
+    <t>Bons du Trésor : actions</t>
+  </si>
+  <si>
+    <t>Obligations à moyen terme actions</t>
+  </si>
+  <si>
+    <t>Obligation à long terme stock</t>
+  </si>
+  <si>
+    <t>Pourcentage de l'action : Bons du Trésor</t>
+  </si>
+  <si>
+    <t>percents</t>
+  </si>
+  <si>
+    <t>Pourcentage de l'action : Obligations à moyen terme</t>
+  </si>
+  <si>
+    <t>Pourcentage de l'action : Obligations à long terme</t>
+  </si>
+  <si>
+    <t>Bons du Trésor arrivant à échéance</t>
+  </si>
+  <si>
+    <t>Montants de la dette arrivant à échéance</t>
+  </si>
+  <si>
+    <t>Obligation de 2 ans expirant</t>
+  </si>
+  <si>
+    <t>Obligation de 3 ans expirant</t>
+  </si>
+  <si>
+    <t>Obligation à 5 ans arrivant à échéance</t>
+  </si>
+  <si>
+    <t>Total de l'obligation MT arrivant à échéance</t>
+  </si>
+  <si>
+    <t>Taux d'intérêt des obligations MT arrivant à échéance</t>
+  </si>
+  <si>
+    <t>Intérêts des obligations MT arrivant à échéance et restantes</t>
+  </si>
+  <si>
+    <t>Taux d'intérêt des obligations MT à durée indéterminée</t>
+  </si>
+  <si>
+    <t>Part des nouvelles obligations à moyen terme</t>
+  </si>
+  <si>
+    <t>Calcul du taux d'intérêt applicable en cours d'exécution</t>
+  </si>
+  <si>
+    <t>Part des nouvelles obligations à long terme</t>
+  </si>
+  <si>
+    <t>Taux d'intérêt applicable à la course à pied : Moyen terme</t>
+  </si>
+  <si>
+    <t>Taux d'intérêt applicable à la course à pied : Long terme</t>
+  </si>
+  <si>
+    <t>Taux d'intérêt applicable à la course à pied : Toutes les dettes</t>
+  </si>
+  <si>
+    <t>The row will appear in either the `input` section, general `outputs` or backend depending of the value specified here.</t>
+  </si>
+  <si>
+    <t>A user visible label in english.</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>A user visible label in French</t>
+  </si>
+  <si>
+    <t>A unique identifier for this aspect. Can be any chain of characters unless the aspect is an input (only letters, underscores and numbers are accepted). Not visible to the end user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> When type is `backend`</t>
+  </si>
+  <si>
+    <t>Aspects will be grouped under this use visible group name. Use the same group name for multiple aspects to group them together.</t>
+  </si>
+  <si>
+    <t>An optional user visible description. Will appear under the aspect label (and unit, if specified) with a gray tone.</t>
+  </si>
+  <si>
+    <t>An optional user visible warning. Will appear under the aspect label, unit (if specified) and description (if specified) with a yellow tone.</t>
+  </si>
+  <si>
+    <t>When TRUE, the values for a given aspect will appear within a grayed out box. Use to display constants and other non-variable values (eg. Imports from an external model).</t>
+  </si>
+  <si>
+    <t>Can be `millions` or `percents`; will be localized to the end user's preference (and multiply values x100 if percents).</t>
+  </si>
+  <si>
+    <t>[Fiscal years]</t>
+  </si>
+  <si>
+    <t>A series of fical year columns must be included. Fiscal year headers MUST adopt the following format: `YYYY-YYYY`.</t>
+  </si>
+  <si>
+    <t>A `machine_readable` sheet must be present and include the fields above.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The field headers MUST be on row 1.</t>
+  </si>
+  <si>
+    <t>Empty rows are not allowed.</t>
+  </si>
+  <si>
+    <t>User inputs should be set to 0 by default.</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -950,7 +1128,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1081,13 +1259,64 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1098,6 +1327,34 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{18D3F2AD-386C-47D7-A08A-D0F9FA78FC08}" name="Table12" displayName="Table12" ref="A1:C14" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C14" xr:uid="{18D3F2AD-386C-47D7-A08A-D0F9FA78FC08}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DC129F0C-83E5-4999-8067-EED30BFDDA18}" name="Field" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E72215B9-C65D-4070-9C6F-FFC8A4850319}" name="Required" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{5E3BB497-0045-4EEA-BCF3-CC45DB3FD769}" name="Description" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{AAB0358D-140B-43B9-A527-231BF75D29FD}" name="Table13" displayName="Table13" ref="C17:C21" totalsRowShown="0">
+  <autoFilter ref="C17:C21" xr:uid="{AAB0358D-140B-43B9-A527-231BF75D29FD}">
+    <filterColumn colId="0" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{3FA4E765-6020-4665-8A64-E72D3247D39B}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1396,25 +1653,215 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08E8843-9E22-442B-AC52-E0B48A2465F9}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="156.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="77" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="77" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="77" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="74" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" s="77" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="77" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="77"/>
+      <c r="C7" s="15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="74" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8" s="77"/>
+      <c r="C8" s="15" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="74" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9" s="77"/>
+      <c r="C9" s="15" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="74" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="77"/>
+      <c r="C10" s="15" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="77"/>
+      <c r="C11" s="15" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="77"/>
+      <c r="C12" s="15" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="74" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="77"/>
+      <c r="C13" s="15" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" s="77"/>
+      <c r="C14" s="15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DA5658-E2EA-4E0B-B547-2D4F388F10E4}">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="73" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="73" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="12" width="25.7109375" customWidth="1"/>
+    <col min="13" max="17" width="9.140625" style="75"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1424,10 +1871,10 @@
       <c r="B1" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="73" t="s">
         <v>197</v>
       </c>
       <c r="E1" t="s">
@@ -1454,19 +1901,19 @@
       <c r="L1" t="s">
         <v>207</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="75" t="s">
         <v>202</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="75" t="s">
         <v>213</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="75" t="s">
         <v>214</v>
       </c>
     </row>
@@ -1493,19 +1940,19 @@
       <c r="L2" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="75">
         <v>1000</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
+      <c r="N2" s="75">
+        <v>0</v>
+      </c>
+      <c r="O2" s="75">
+        <v>0</v>
+      </c>
+      <c r="P2" s="75">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="75">
         <v>0</v>
       </c>
     </row>
@@ -1532,19 +1979,19 @@
       <c r="L3" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
+      <c r="M3" s="75">
+        <v>0</v>
+      </c>
+      <c r="N3" s="75">
+        <v>5</v>
+      </c>
+      <c r="O3" s="75">
+        <v>0</v>
+      </c>
+      <c r="P3" s="75">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="75">
         <v>0</v>
       </c>
     </row>
@@ -1571,25 +2018,25 @@
       <c r="L4" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="75">
         <f>'For user (EN)'!C10</f>
         <v>36.021489692499657</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="75">
         <f>'For user (EN)'!D10</f>
-        <v>37.319037412166516</v>
-      </c>
-      <c r="O4">
+        <v>37.182973343026013</v>
+      </c>
+      <c r="O4" s="75">
         <f>'For user (EN)'!E10</f>
-        <v>29.208615938255132</v>
-      </c>
-      <c r="P4">
+        <v>29.068849182932411</v>
+      </c>
+      <c r="P4" s="75">
         <f>'For user (EN)'!F10</f>
-        <v>30.003464565959376</v>
-      </c>
-      <c r="Q4">
+        <v>29.859894363944697</v>
+      </c>
+      <c r="Q4" s="75">
         <f>'For user (EN)'!G10</f>
-        <v>30.819943261390854</v>
+        <v>30.672466110197487</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1615,25 +2062,25 @@
       <c r="L5" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="75">
         <f>'For user (EN)'!C11</f>
         <v>1036.0214896924997</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="75">
         <f>'For user (EN)'!D11</f>
-        <v>1073.3405271046663</v>
-      </c>
-      <c r="O5">
+        <v>1068.2044630355258</v>
+      </c>
+      <c r="O5" s="75">
         <f>'For user (EN)'!E11</f>
-        <v>1102.5491430429215</v>
-      </c>
-      <c r="P5">
+        <v>1097.2733122184582</v>
+      </c>
+      <c r="P5" s="75">
         <f>'For user (EN)'!F11</f>
-        <v>1132.5526076088809</v>
-      </c>
-      <c r="Q5">
+        <v>1127.1332065824029</v>
+      </c>
+      <c r="Q5" s="75">
         <f>'For user (EN)'!G11</f>
-        <v>1163.3725508702717</v>
+        <v>1157.8056726926004</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="120" x14ac:dyDescent="0.25">
@@ -1663,25 +2110,25 @@
       <c r="L6" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="75">
         <f>'For user (EN)'!C12</f>
         <v>1036.0214896924997</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="75">
         <f>'For user (EN)'!D12</f>
-        <v>37.319037412166516</v>
-      </c>
-      <c r="O6">
+        <v>32.182973343026013</v>
+      </c>
+      <c r="O6" s="75">
         <f>'For user (EN)'!E12</f>
-        <v>29.208615938255132</v>
-      </c>
-      <c r="P6">
+        <v>29.068849182932411</v>
+      </c>
+      <c r="P6" s="75">
         <f>'For user (EN)'!F12</f>
-        <v>30.003464565959376</v>
-      </c>
-      <c r="Q6">
+        <v>29.859894363944697</v>
+      </c>
+      <c r="Q6" s="75">
         <f>'For user (EN)'!G12</f>
-        <v>30.819943261390854</v>
+        <v>30.672466110197487</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1707,25 +2154,25 @@
       <c r="L7" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="75">
         <f>'For user (EN)'!C13</f>
         <v>36.021489692499657</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="75">
         <f>'For user (EN)'!D13</f>
-        <v>73.340527104666165</v>
-      </c>
-      <c r="O7">
+        <v>73.204463035525663</v>
+      </c>
+      <c r="O7" s="75">
         <f>'For user (EN)'!E13</f>
-        <v>102.5491430429213</v>
-      </c>
-      <c r="P7">
+        <v>102.27331221845807</v>
+      </c>
+      <c r="P7" s="75">
         <f>'For user (EN)'!F13</f>
-        <v>132.55260760888069</v>
-      </c>
-      <c r="Q7">
+        <v>132.13320658240278</v>
+      </c>
+      <c r="Q7" s="75">
         <f>'For user (EN)'!G13</f>
-        <v>163.37255087027154</v>
+        <v>162.80567269260027</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1755,23 +2202,23 @@
         <v>1</v>
       </c>
       <c r="L8" s="15"/>
-      <c r="M8" s="24">
+      <c r="M8" s="75">
         <f>Model!D10</f>
         <v>3.7</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="75">
         <f>Model!E10</f>
         <v>2.4500000000000002</v>
       </c>
-      <c r="O8" s="24">
+      <c r="O8" s="75">
         <f>Model!F10</f>
         <v>2.4500000000000002</v>
       </c>
-      <c r="P8" s="24">
+      <c r="P8" s="75">
         <f>Model!G10</f>
         <v>2.4500000000000002</v>
       </c>
-      <c r="Q8" s="24">
+      <c r="Q8" s="75">
         <f>Model!H10</f>
         <v>2.4500000000000002</v>
       </c>
@@ -1803,293 +2250,952 @@
         <v>1</v>
       </c>
       <c r="L9" s="15"/>
-      <c r="M9" s="24">
+      <c r="M9" s="75">
         <f>Model!D11</f>
         <v>3.5207104999999999</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="75">
         <f>Model!E11</f>
         <v>3.5</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9" s="75">
         <f>Model!F11</f>
         <v>3.5</v>
       </c>
-      <c r="P9" s="24">
+      <c r="P9" s="75">
         <f>Model!G11</f>
         <v>3.5</v>
       </c>
-      <c r="Q9" s="24">
+      <c r="Q9" s="75">
         <f>Model!H11</f>
         <v>3.5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>232</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>226</v>
+      </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="K10" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="M10" s="75">
+        <f>Model!D12</f>
+        <v>3.4672898500000002</v>
+      </c>
+      <c r="N10" s="75">
+        <f>Model!E12</f>
+        <v>2.93</v>
+      </c>
+      <c r="O10" s="75">
+        <f>Model!F12</f>
+        <v>2.93</v>
+      </c>
+      <c r="P10" s="75">
+        <f>Model!G12</f>
+        <v>2.93</v>
+      </c>
+      <c r="Q10" s="75">
+        <f>Model!H12</f>
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>233</v>
+      </c>
+      <c r="D11" s="73" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>226</v>
+      </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
+      <c r="K11" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="M11" s="75">
+        <f>Model!D13</f>
+        <v>3.6021489692499662</v>
+      </c>
+      <c r="N11" s="75">
+        <f>Model!E13</f>
+        <v>2.7212813828101048</v>
+      </c>
+      <c r="O11" s="75">
+        <f>Model!F13</f>
+        <v>2.7212813828101048</v>
+      </c>
+      <c r="P11" s="75">
+        <f>Model!G13</f>
+        <v>2.7212813828101048</v>
+      </c>
+      <c r="Q11" s="75">
+        <f>Model!H13</f>
+        <v>2.7212813828101048</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>236</v>
+      </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="M12" s="75">
+        <f>Model!D16</f>
+        <v>36.021489692499657</v>
+      </c>
+      <c r="N12" s="75">
+        <f>Model!E16</f>
+        <v>-0.13606406914050523</v>
+      </c>
+      <c r="O12" s="75">
+        <f>Model!F16</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="75">
+        <f>Model!G16</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="75">
+        <f>Model!H16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="73" t="s">
+        <v>238</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>236</v>
+      </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="M13" s="75">
+        <f>Model!D17</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="75">
+        <f>Model!E17</f>
+        <v>37.319037412166516</v>
+      </c>
+      <c r="O13" s="75">
+        <f>Model!F17</f>
+        <v>29.068849182932411</v>
+      </c>
+      <c r="P13" s="75">
+        <f>Model!G17</f>
+        <v>29.859894363944697</v>
+      </c>
+      <c r="Q13" s="75">
+        <f>Model!H17</f>
+        <v>30.672466110197487</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>236</v>
+      </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="M14" s="75">
+        <f>Model!D18</f>
+        <v>-1036.0214896924997</v>
+      </c>
+      <c r="N14" s="75">
+        <f>Model!E18</f>
+        <v>-32.182973343026013</v>
+      </c>
+      <c r="O14" s="75">
+        <f>Model!F18</f>
+        <v>-29.068849182932411</v>
+      </c>
+      <c r="P14" s="75">
+        <f>Model!G18</f>
+        <v>-29.859894363944697</v>
+      </c>
+      <c r="Q14" s="75">
+        <f>Model!H18</f>
+        <v>-30.672466110197487</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>236</v>
+      </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="M15" s="75">
+        <f>Model!D19</f>
+        <v>-1036.0214896924997</v>
+      </c>
+      <c r="N15" s="75">
+        <f>Model!E19</f>
+        <v>-1068.2044630355258</v>
+      </c>
+      <c r="O15" s="75">
+        <f>Model!F19</f>
+        <v>-1097.2733122184582</v>
+      </c>
+      <c r="P15" s="75">
+        <f>Model!G19</f>
+        <v>-1127.1332065824029</v>
+      </c>
+      <c r="Q15" s="75">
+        <f>Model!H19</f>
+        <v>-1157.8056726926004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="M16" s="75">
+        <f>Model!D22</f>
+        <v>-576.1076583314034</v>
+      </c>
+      <c r="N16" s="75">
+        <f>Model!E22</f>
+        <v>-17.896209292237543</v>
+      </c>
+      <c r="O16" s="75">
+        <f>Model!F22</f>
+        <v>-16.164516662814123</v>
+      </c>
+      <c r="P16" s="75">
+        <f>Model!G22</f>
+        <v>-16.60439864538052</v>
+      </c>
+      <c r="Q16" s="75">
+        <f>Model!H22</f>
+        <v>-17.056251054444832</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" s="73" t="s">
+        <v>244</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="M17" s="75">
+        <f>Model!D23</f>
+        <v>-354.13365014804413</v>
+      </c>
+      <c r="N17" s="75">
+        <f>Model!E23</f>
+        <v>-11.000808319107122</v>
+      </c>
+      <c r="O17" s="75">
+        <f>Model!F23</f>
+        <v>-9.9363360404910814</v>
+      </c>
+      <c r="P17" s="75">
+        <f>Model!G23</f>
+        <v>-10.206731703294416</v>
+      </c>
+      <c r="Q17" s="75">
+        <f>Model!H23</f>
+        <v>-10.484485592929543</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="73" t="s">
+        <v>245</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="M18" s="75">
+        <f>Model!D24</f>
+        <v>-105.78018121305216</v>
+      </c>
+      <c r="N18" s="75">
+        <f>Model!E24</f>
+        <v>-3.2859557316813484</v>
+      </c>
+      <c r="O18" s="75">
+        <f>Model!F24</f>
+        <v>-2.9679964796272067</v>
+      </c>
+      <c r="P18" s="75">
+        <f>Model!G24</f>
+        <v>-3.0487640152697613</v>
+      </c>
+      <c r="Q18" s="75">
+        <f>Model!H24</f>
+        <v>-3.1317294628231109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="M19" s="75">
+        <f>Model!D25</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="75">
+        <f>Model!E25</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="75">
+        <f>Model!F25</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="75">
+        <f>Model!G25</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="75">
+        <f>Model!H25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="M20" s="75">
+        <f>Model!D26</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="75">
+        <f>Model!E26</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="75">
+        <f>Model!F26</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="75">
+        <f>Model!G26</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="75">
+        <f>Model!H26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C21" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="73" t="s">
+        <v>248</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="M21" s="75">
+        <f>Model!D27</f>
+        <v>-576.1076583314034</v>
+      </c>
+      <c r="N21" s="75">
+        <f>Model!E27</f>
+        <v>-594.00386762364099</v>
+      </c>
+      <c r="O21" s="75">
+        <f>Model!F27</f>
+        <v>-610.16838428645508</v>
+      </c>
+      <c r="P21" s="75">
+        <f>Model!G27</f>
+        <v>-626.77278293183565</v>
+      </c>
+      <c r="Q21" s="75">
+        <f>Model!H27</f>
+        <v>-643.82903398628048</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C22" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="73" t="s">
+        <v>249</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="M22" s="75">
+        <f>Model!D28</f>
+        <v>-354.13365014804413</v>
+      </c>
+      <c r="N22" s="75">
+        <f>Model!E28</f>
+        <v>-365.13445846715126</v>
+      </c>
+      <c r="O22" s="75">
+        <f>Model!F28</f>
+        <v>-375.07079450764235</v>
+      </c>
+      <c r="P22" s="75">
+        <f>Model!G28</f>
+        <v>-385.27752621093674</v>
+      </c>
+      <c r="Q22" s="75">
+        <f>Model!H28</f>
+        <v>-395.7620118038663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="73" t="s">
+        <v>250</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+      <c r="M23" s="75">
+        <f>Model!D29</f>
+        <v>-105.78018121305216</v>
+      </c>
+      <c r="N23" s="75">
+        <f>Model!E29</f>
+        <v>-109.06613694473351</v>
+      </c>
+      <c r="O23" s="75">
+        <f>Model!F29</f>
+        <v>-112.03413342436072</v>
+      </c>
+      <c r="P23" s="75">
+        <f>Model!G29</f>
+        <v>-115.08289743963047</v>
+      </c>
+      <c r="Q23" s="75">
+        <f>Model!H29</f>
+        <v>-118.21462690245359</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C24" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>251</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="L24" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="M24" s="75">
+        <f>Model!D30</f>
+        <v>0.55607693861871266</v>
+      </c>
+      <c r="N24" s="75">
+        <f>Model!E30</f>
+        <v>0.55607693861871266</v>
+      </c>
+      <c r="O24" s="75">
+        <f>Model!F30</f>
+        <v>0.55607693861871266</v>
+      </c>
+      <c r="P24" s="75">
+        <f>Model!G30</f>
+        <v>0.55607693861871266</v>
+      </c>
+      <c r="Q24" s="75">
+        <f>Model!H30</f>
+        <v>0.55607693861871266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" s="73" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>253</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="15"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="L25" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="M25" s="75">
+        <f>Model!D31</f>
+        <v>0.34182075726359124</v>
+      </c>
+      <c r="N25" s="75">
+        <f>Model!E31</f>
+        <v>0.34182075726359124</v>
+      </c>
+      <c r="O25" s="75">
+        <f>Model!F31</f>
+        <v>0.34182075726359124</v>
+      </c>
+      <c r="P25" s="75">
+        <f>Model!G31</f>
+        <v>0.34182075726359124</v>
+      </c>
+      <c r="Q25" s="75">
+        <f>Model!H31</f>
+        <v>0.34182075726359124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" s="73" t="s">
+        <v>254</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>243</v>
+      </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="L26" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="M26" s="75">
+        <f>Model!D32</f>
+        <v>0.10210230411769609</v>
+      </c>
+      <c r="N26" s="75">
+        <f>Model!E32</f>
+        <v>0.10210230411769609</v>
+      </c>
+      <c r="O26" s="75">
+        <f>Model!F32</f>
+        <v>0.10210230411769609</v>
+      </c>
+      <c r="P26" s="75">
+        <f>Model!G32</f>
+        <v>0.10210230411769609</v>
+      </c>
+      <c r="Q26" s="75">
+        <f>Model!H32</f>
+        <v>0.10210230411769609</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C27" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>256</v>
+      </c>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
+      <c r="N27" s="75">
+        <f>Model!E35</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="75">
+        <f>Model!F35</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="75">
+        <f>Model!G35</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="75">
+        <f>Model!H35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C28" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="73" t="s">
+        <v>257</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>256</v>
+      </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="15"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="O28" s="75">
+        <f>Model!F36</f>
+        <v>0</v>
+      </c>
+      <c r="P28" s="75">
+        <f>Model!G36</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="75">
+        <f>Model!H36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C29" s="73" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>256</v>
+      </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="15"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="P29" s="75">
+        <f>Model!G37</f>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="75">
+        <f>Model!H37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>256</v>
+      </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
@@ -2097,83 +3203,345 @@
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="15"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
+    <row r="31" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="73" t="s">
+        <v>260</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>256</v>
+      </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="15"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
+      <c r="O31" s="75">
+        <f>Model!F39</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="75">
+        <f>Model!G39</f>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="75">
+        <f>Model!H39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" s="73" t="s">
+        <v>159</v>
+      </c>
+      <c r="D32" s="73" t="s">
+        <v>261</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>262</v>
+      </c>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="15"/>
-      <c r="C33" s="73"/>
-      <c r="D33" s="73"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
+      <c r="O32" s="24">
+        <f>Model!F41</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="24">
+        <f>Model!G41</f>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="24">
+        <f>Model!H41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" s="73" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="73" t="s">
+        <v>263</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>262</v>
+      </c>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="15"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
+      <c r="N33" s="24">
+        <f>Model!E42</f>
+        <v>2.93</v>
+      </c>
+      <c r="O33" s="24">
+        <f>Model!F42</f>
+        <v>2.93</v>
+      </c>
+      <c r="P33" s="24">
+        <f>Model!G42</f>
+        <v>2.93</v>
+      </c>
+      <c r="Q33" s="24">
+        <f>Model!H42</f>
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C34" s="73" t="s">
+        <v>180</v>
+      </c>
+      <c r="D34" s="73" t="s">
+        <v>264</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>265</v>
+      </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="15"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+      <c r="L34" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="M34" s="20">
+        <f>Model!D45</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="20">
+        <f>Model!E45</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="20">
+        <f>Model!F45</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="20">
+        <f>Model!G45</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="20">
+        <f>Model!H45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C35" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="D35" s="73" t="s">
+        <v>266</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>265</v>
+      </c>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="15"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="L35" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="M35" s="76">
+        <f>Model!D46</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="76">
+        <f>Model!E46</f>
+        <v>0</v>
+      </c>
+      <c r="O35" s="76">
+        <f>Model!F46</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="76">
+        <f>Model!G46</f>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="76">
+        <f>Model!H46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C36" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="73" t="s">
+        <v>267</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>265</v>
+      </c>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
+      <c r="M36" s="24">
+        <f>Model!D47</f>
+        <v>3.4672898500000002</v>
+      </c>
+      <c r="N36" s="24">
+        <f>Model!E47</f>
+        <v>2.93</v>
+      </c>
+      <c r="O36" s="24">
+        <f>Model!F47</f>
+        <v>2.93</v>
+      </c>
+      <c r="P36" s="24">
+        <f>Model!G47</f>
+        <v>2.93</v>
+      </c>
+      <c r="Q36" s="24">
+        <f>Model!H47</f>
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C37" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="73" t="s">
+        <v>268</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="M37" s="24">
+        <f>Model!D48</f>
+        <v>3.5207104999999999</v>
+      </c>
+      <c r="N37" s="24">
+        <f>Model!E48</f>
+        <v>3.5</v>
+      </c>
+      <c r="O37" s="24">
+        <f>Model!F48</f>
+        <v>3.5</v>
+      </c>
+      <c r="P37" s="24">
+        <f>Model!G48</f>
+        <v>3.5</v>
+      </c>
+      <c r="Q37" s="24">
+        <f>Model!H48</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C38" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="73" t="s">
+        <v>269</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="M38" s="24">
+        <f>Model!D50</f>
+        <v>3.6021489692499662</v>
+      </c>
+      <c r="N38" s="24">
+        <f>Model!E50</f>
+        <v>2.7212813828101048</v>
+      </c>
+      <c r="O38" s="24">
+        <f>Model!F50</f>
+        <v>2.7212813828101048</v>
+      </c>
+      <c r="P38" s="24">
+        <f>Model!G50</f>
+        <v>2.7212813828101048</v>
+      </c>
+      <c r="Q38" s="24">
+        <f>Model!H50</f>
+        <v>2.7212813828101048</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2181,7 +3549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8F7545-787E-47D5-A81D-527FE013B894}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -2295,7 +3663,7 @@
       </c>
       <c r="D5" s="4">
         <f>machine_readable!N3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="4">
         <f>machine_readable!O3</f>
@@ -2323,7 +3691,7 @@
       </c>
       <c r="D6" s="68">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E6" s="68">
         <f t="shared" si="2"/>
@@ -2362,19 +3730,19 @@
       </c>
       <c r="D10" s="13">
         <f>Model!E53</f>
-        <v>37.319037412166516</v>
+        <v>37.182973343026013</v>
       </c>
       <c r="E10" s="13">
         <f>Model!F53</f>
-        <v>29.208615938255132</v>
+        <v>29.068849182932411</v>
       </c>
       <c r="F10" s="13">
         <f>Model!G53</f>
-        <v>30.003464565959376</v>
+        <v>29.859894363944697</v>
       </c>
       <c r="G10" s="13">
         <f>Model!H53</f>
-        <v>30.819943261390854</v>
+        <v>30.672466110197487</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2390,19 +3758,19 @@
       </c>
       <c r="D11" s="13">
         <f>Model!E54</f>
-        <v>1073.3405271046663</v>
+        <v>1068.2044630355258</v>
       </c>
       <c r="E11" s="13">
         <f>Model!F54</f>
-        <v>1102.5491430429215</v>
+        <v>1097.2733122184582</v>
       </c>
       <c r="F11" s="13">
         <f>Model!G54</f>
-        <v>1132.5526076088809</v>
+        <v>1127.1332065824029</v>
       </c>
       <c r="G11" s="13">
         <f>Model!H54</f>
-        <v>1163.3725508702717</v>
+        <v>1157.8056726926004</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2418,19 +3786,19 @@
       </c>
       <c r="D12" s="13">
         <f>Model!E53+Model!E6</f>
-        <v>37.319037412166516</v>
+        <v>32.182973343026013</v>
       </c>
       <c r="E12" s="13">
         <f>Model!F53+Model!F6</f>
-        <v>29.208615938255132</v>
+        <v>29.068849182932411</v>
       </c>
       <c r="F12" s="13">
         <f>Model!G53+Model!G6</f>
-        <v>30.003464565959376</v>
+        <v>29.859894363944697</v>
       </c>
       <c r="G12" s="13">
         <f>Model!H53+Model!H6</f>
-        <v>30.819943261390854</v>
+        <v>30.672466110197487</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2446,19 +3814,19 @@
       </c>
       <c r="D13" s="51">
         <f>SUM($C10:D10)</f>
-        <v>73.340527104666165</v>
+        <v>73.204463035525663</v>
       </c>
       <c r="E13" s="51">
         <f>SUM($C10:E10)</f>
-        <v>102.5491430429213</v>
+        <v>102.27331221845807</v>
       </c>
       <c r="F13" s="51">
         <f>SUM($C10:F10)</f>
-        <v>132.55260760888069</v>
+        <v>132.13320658240278</v>
       </c>
       <c r="G13" s="51">
         <f>SUM($C10:G10)</f>
-        <v>163.37255087027154</v>
+        <v>162.80567269260027</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2481,15 +3849,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB77E90E-259F-4B12-BB0C-68506FD8C7E4}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,7 +3971,7 @@
       </c>
       <c r="E5" s="68">
         <f>'For user (EN)'!D5</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F5" s="68">
         <f>'For user (EN)'!E5</f>
@@ -2632,7 +4000,7 @@
       </c>
       <c r="E6" s="68">
         <f>'For user (EN)'!D6</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="F6" s="68">
         <f>'For user (EN)'!E6</f>
@@ -2823,7 +4191,7 @@
       </c>
       <c r="E16" s="9">
         <f>(E13/100)*E6</f>
-        <v>0</v>
+        <v>-0.13606406914050523</v>
       </c>
       <c r="F16" s="9">
         <f t="shared" ref="F16:H16" si="1">(F13/100)*F6</f>
@@ -2856,15 +4224,15 @@
       </c>
       <c r="F17" s="9">
         <f>(E50/100)*E54</f>
-        <v>29.208615938255132</v>
+        <v>29.068849182932411</v>
       </c>
       <c r="G17" s="9">
         <f>(F50/100)*F54</f>
-        <v>30.003464565959376</v>
+        <v>29.859894363944697</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" ref="H17" si="2">(G50/100)*G54</f>
-        <v>30.819943261390854</v>
+        <v>30.672466110197487</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -2881,19 +4249,19 @@
       </c>
       <c r="E18" s="9">
         <f>-(E6+E16+E17)</f>
-        <v>-37.319037412166516</v>
+        <v>-32.182973343026013</v>
       </c>
       <c r="F18" s="9">
         <f>-(F6+F16+F17)</f>
-        <v>-29.208615938255132</v>
+        <v>-29.068849182932411</v>
       </c>
       <c r="G18" s="9">
         <f>-(G6+G16+G17)</f>
-        <v>-30.003464565959376</v>
+        <v>-29.859894363944697</v>
       </c>
       <c r="H18" s="9">
         <f t="shared" ref="H18" si="3">-(H6+H16+H17)</f>
-        <v>-30.819943261390854</v>
+        <v>-30.672466110197487</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2910,19 +4278,19 @@
       </c>
       <c r="E19" s="9">
         <f>SUM($D18:E18)</f>
-        <v>-1073.3405271046663</v>
+        <v>-1068.2044630355258</v>
       </c>
       <c r="F19" s="9">
         <f>SUM($D18:F18)</f>
-        <v>-1102.5491430429215</v>
+        <v>-1097.2733122184582</v>
       </c>
       <c r="G19" s="9">
         <f>SUM($D18:G18)</f>
-        <v>-1132.5526076088809</v>
+        <v>-1127.1332065824029</v>
       </c>
       <c r="H19" s="9">
         <f>SUM($D18:H18)</f>
-        <v>-1163.3725508702717</v>
+        <v>-1157.8056726926004</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2961,19 +4329,19 @@
       </c>
       <c r="E22" s="9">
         <f>SUM(E18,E35,E39)*'Fiscal Model Import'!F2</f>
-        <v>-20.752256076354762</v>
+        <v>-17.896209292237543</v>
       </c>
       <c r="F22" s="9">
         <f>SUM(F18,F35,F39)*'Fiscal Model Import'!G2</f>
-        <v>-16.242237732234653</v>
+        <v>-16.164516662814123</v>
       </c>
       <c r="G22" s="9">
         <f>SUM(G18,G35,G39)*'Fiscal Model Import'!H2</f>
-        <v>-16.684234723793711</v>
+        <v>-16.60439864538052</v>
       </c>
       <c r="H22" s="9">
         <f>SUM(H18,H35,H39)*'Fiscal Model Import'!I2</f>
-        <v>-17.138259697196649</v>
+        <v>-17.056251054444832</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -2990,19 +4358,19 @@
       </c>
       <c r="E23" s="69">
         <f>SUM(E18,E35,E39)*'Fiscal Model Import'!F4</f>
-        <v>-12.756421628575051</v>
+        <v>-11.000808319107122</v>
       </c>
       <c r="F23" s="69">
         <f>SUM(F18,F35,F39)*'Fiscal Model Import'!G4</f>
-        <v>-9.9841112186357694</v>
+        <v>-9.9363360404910814</v>
       </c>
       <c r="G23" s="69">
         <f>SUM(G18,G35,G39)*'Fiscal Model Import'!H4</f>
-        <v>-10.255806978467561</v>
+        <v>-10.206731703294416</v>
       </c>
       <c r="H23" s="69">
         <f>SUM(H18,H35,H39)*'Fiscal Model Import'!I4</f>
-        <v>-10.534896344429537</v>
+        <v>-10.484485592929543</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -3019,19 +4387,19 @@
       </c>
       <c r="E24" s="69">
         <f>SUM(E18,E35,E39)*'Fiscal Model Import'!F3</f>
-        <v>-3.8103597072367039</v>
+        <v>-3.2859557316813484</v>
       </c>
       <c r="F24" s="69">
         <f>SUM(F18,F35,F39)*'Fiscal Model Import'!G3</f>
-        <v>-2.982266987384711</v>
+        <v>-2.9679964796272067</v>
       </c>
       <c r="G24" s="69">
         <f>SUM(G18,G35,G39)*'Fiscal Model Import'!H3</f>
-        <v>-3.0634228636981029</v>
+        <v>-3.0487640152697613</v>
       </c>
       <c r="H24" s="69">
         <f>SUM(H18,H35,H39)*'Fiscal Model Import'!I3</f>
-        <v>-3.1467872197646676</v>
+        <v>-3.1317294628231109</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3106,19 +4474,19 @@
       </c>
       <c r="E27" s="69">
         <f>IF(AND(SUM(E$18,E$35,E$39)&gt;0,E19&gt;0),D27+E22-E35,E$19*D30)</f>
-        <v>-596.8599144077582</v>
+        <v>-594.00386762364099</v>
       </c>
       <c r="F27" s="69">
         <f>IF(AND(SUM(F$18,F$35,F$39)&gt;0,F19&gt;0),E27+F22-F35,F$19*E30)</f>
-        <v>-613.10215213999288</v>
+        <v>-610.16838428645508</v>
       </c>
       <c r="G27" s="69">
         <f t="shared" ref="G27:H27" si="4">IF(AND(SUM(G$18,G$35,G$39)&gt;0,G19&gt;0),F27+G22-G35,G$19*F30)</f>
-        <v>-629.78638686378656</v>
+        <v>-626.77278293183565</v>
       </c>
       <c r="H27" s="69">
         <f t="shared" si="4"/>
-        <v>-646.92464656098321</v>
+        <v>-643.82903398628048</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -3135,19 +4503,19 @@
       </c>
       <c r="E28" s="69">
         <f>IF(AND(SUM(E$18,E$35,E$39)&gt;0,E19&gt;0),D28+E23-E39,E$19*D31)</f>
-        <v>-366.89007177661921</v>
+        <v>-365.13445846715126</v>
       </c>
       <c r="F28" s="69">
         <f t="shared" ref="F28:H28" si="5">IF(AND(SUM(F$18,F$35,F$39)&gt;0,F19&gt;0),E28+F23-F39,F$19*E31)</f>
-        <v>-376.87418299525501</v>
+        <v>-375.07079450764235</v>
       </c>
       <c r="G28" s="69">
         <f t="shared" si="5"/>
-        <v>-387.12998997372256</v>
+        <v>-385.27752621093674</v>
       </c>
       <c r="H28" s="69">
         <f t="shared" si="5"/>
-        <v>-397.66488631815207</v>
+        <v>-395.7620118038663</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -3164,19 +4532,19 @@
       </c>
       <c r="E29" s="69">
         <f>IF(AND(SUM(E$18,E$35,E$39)&gt;0,E19&gt;0),D29+E24,E$19*D32)</f>
-        <v>-109.59054092028887</v>
+        <v>-109.06613694473351</v>
       </c>
       <c r="F29" s="69">
         <f t="shared" ref="F29:H29" si="6">IF(AND(SUM(F$18,F$35,F$39)&gt;0,F19&gt;0),E29+F24,F$19*E32)</f>
-        <v>-112.57280790767358</v>
+        <v>-112.03413342436072</v>
       </c>
       <c r="G29" s="69">
         <f t="shared" si="6"/>
-        <v>-115.63623077137169</v>
+        <v>-115.08289743963047</v>
       </c>
       <c r="H29" s="69">
         <f t="shared" si="6"/>
-        <v>-118.78301799113635</v>
+        <v>-118.21462690245359</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3659,19 +5027,19 @@
       </c>
       <c r="E53" s="13">
         <f>E16+E17</f>
-        <v>37.319037412166516</v>
+        <v>37.182973343026013</v>
       </c>
       <c r="F53" s="13">
         <f>F16+F17</f>
-        <v>29.208615938255132</v>
+        <v>29.068849182932411</v>
       </c>
       <c r="G53" s="13">
         <f t="shared" ref="G53:H53" si="18">G16+G17</f>
-        <v>30.003464565959376</v>
+        <v>29.859894363944697</v>
       </c>
       <c r="H53" s="13">
         <f t="shared" si="18"/>
-        <v>30.819943261390854</v>
+        <v>30.672466110197487</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3686,19 +5054,19 @@
       </c>
       <c r="E54" s="13">
         <f t="shared" si="19"/>
-        <v>1073.3405271046663</v>
+        <v>1068.2044630355258</v>
       </c>
       <c r="F54" s="13">
         <f t="shared" si="19"/>
-        <v>1102.5491430429215</v>
+        <v>1097.2733122184582</v>
       </c>
       <c r="G54" s="13">
         <f t="shared" si="19"/>
-        <v>1132.5526076088809</v>
+        <v>1127.1332065824029</v>
       </c>
       <c r="H54" s="13">
         <f t="shared" si="19"/>
-        <v>1163.3725508702717</v>
+        <v>1157.8056726926004</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3713,19 +5081,19 @@
       </c>
       <c r="E55" s="13">
         <f>SUM($D53:E53)</f>
-        <v>73.340527104666165</v>
+        <v>73.204463035525663</v>
       </c>
       <c r="F55" s="13">
         <f>SUM($D53:F53)</f>
-        <v>102.5491430429213</v>
+        <v>102.27331221845807</v>
       </c>
       <c r="G55" s="13">
         <f>SUM($D53:G53)</f>
-        <v>132.55260760888069</v>
+        <v>132.13320658240278</v>
       </c>
       <c r="H55" s="13">
         <f>SUM($D53:H53)</f>
-        <v>163.37255087027154</v>
+        <v>162.80567269260027</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3752,7 +5120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74A8114-85A4-4459-AF2E-EB80FAA87B37}">
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
@@ -6648,7 +8016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED5BD51-C573-4F48-97F2-040C756B17DC}">
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>

</xml_diff>

<commit_message>
Debug bar is more useful.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\WORKDIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF752891-D999-47CC-8055-575D0199C694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39D5111-2DEA-4D3B-A05A-FB114E8F5855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-3285" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
+    <workbookView xWindow="-28920" yWindow="-3285" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
   </bookViews>
   <sheets>
     <sheet name="How to interface with Web tool" sheetId="8" r:id="rId1"/>
@@ -1845,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DA5658-E2EA-4E0B-B547-2D4F388F10E4}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,7 +1941,7 @@
         <v>211</v>
       </c>
       <c r="M2" s="75">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N2" s="75">
         <v>0</v>
@@ -1983,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="75">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O3" s="75">
         <v>0</v>
@@ -2020,23 +2020,23 @@
       </c>
       <c r="M4" s="75">
         <f>'For user (EN)'!C10</f>
-        <v>36.021489692499657</v>
+        <v>0</v>
       </c>
       <c r="N4" s="75">
         <f>'For user (EN)'!D10</f>
-        <v>37.182973343026013</v>
+        <v>0</v>
       </c>
       <c r="O4" s="75">
         <f>'For user (EN)'!E10</f>
-        <v>29.068849182932411</v>
+        <v>0</v>
       </c>
       <c r="P4" s="75">
         <f>'For user (EN)'!F10</f>
-        <v>29.859894363944697</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="75">
         <f>'For user (EN)'!G10</f>
-        <v>30.672466110197487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2064,23 +2064,23 @@
       </c>
       <c r="M5" s="75">
         <f>'For user (EN)'!C11</f>
-        <v>1036.0214896924997</v>
+        <v>0</v>
       </c>
       <c r="N5" s="75">
         <f>'For user (EN)'!D11</f>
-        <v>1068.2044630355258</v>
+        <v>0</v>
       </c>
       <c r="O5" s="75">
         <f>'For user (EN)'!E11</f>
-        <v>1097.2733122184582</v>
+        <v>0</v>
       </c>
       <c r="P5" s="75">
         <f>'For user (EN)'!F11</f>
-        <v>1127.1332065824029</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="75">
         <f>'For user (EN)'!G11</f>
-        <v>1157.8056726926004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="120" x14ac:dyDescent="0.25">
@@ -2112,23 +2112,23 @@
       </c>
       <c r="M6" s="75">
         <f>'For user (EN)'!C12</f>
-        <v>1036.0214896924997</v>
+        <v>0</v>
       </c>
       <c r="N6" s="75">
         <f>'For user (EN)'!D12</f>
-        <v>32.182973343026013</v>
+        <v>0</v>
       </c>
       <c r="O6" s="75">
         <f>'For user (EN)'!E12</f>
-        <v>29.068849182932411</v>
+        <v>0</v>
       </c>
       <c r="P6" s="75">
         <f>'For user (EN)'!F12</f>
-        <v>29.859894363944697</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="75">
         <f>'For user (EN)'!G12</f>
-        <v>30.672466110197487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2156,23 +2156,23 @@
       </c>
       <c r="M7" s="75">
         <f>'For user (EN)'!C13</f>
-        <v>36.021489692499657</v>
+        <v>0</v>
       </c>
       <c r="N7" s="75">
         <f>'For user (EN)'!D13</f>
-        <v>73.204463035525663</v>
+        <v>0</v>
       </c>
       <c r="O7" s="75">
         <f>'For user (EN)'!E13</f>
-        <v>102.27331221845807</v>
+        <v>0</v>
       </c>
       <c r="P7" s="75">
         <f>'For user (EN)'!F13</f>
-        <v>132.13320658240278</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="75">
         <f>'For user (EN)'!G13</f>
-        <v>162.80567269260027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2394,11 +2394,11 @@
       <c r="L12" s="15"/>
       <c r="M12" s="75">
         <f>Model!D16</f>
-        <v>36.021489692499657</v>
+        <v>0</v>
       </c>
       <c r="N12" s="75">
         <f>Model!E16</f>
-        <v>-0.13606406914050523</v>
+        <v>0</v>
       </c>
       <c r="O12" s="75">
         <f>Model!F16</f>
@@ -2444,19 +2444,19 @@
       </c>
       <c r="N13" s="75">
         <f>Model!E17</f>
-        <v>37.319037412166516</v>
+        <v>0</v>
       </c>
       <c r="O13" s="75">
         <f>Model!F17</f>
-        <v>29.068849182932411</v>
+        <v>0</v>
       </c>
       <c r="P13" s="75">
         <f>Model!G17</f>
-        <v>29.859894363944697</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="75">
         <f>Model!H17</f>
-        <v>30.672466110197487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2486,23 +2486,23 @@
       <c r="L14" s="15"/>
       <c r="M14" s="75">
         <f>Model!D18</f>
-        <v>-1036.0214896924997</v>
+        <v>0</v>
       </c>
       <c r="N14" s="75">
         <f>Model!E18</f>
-        <v>-32.182973343026013</v>
+        <v>0</v>
       </c>
       <c r="O14" s="75">
         <f>Model!F18</f>
-        <v>-29.068849182932411</v>
+        <v>0</v>
       </c>
       <c r="P14" s="75">
         <f>Model!G18</f>
-        <v>-29.859894363944697</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="75">
         <f>Model!H18</f>
-        <v>-30.672466110197487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2532,23 +2532,23 @@
       <c r="L15" s="15"/>
       <c r="M15" s="75">
         <f>Model!D19</f>
-        <v>-1036.0214896924997</v>
+        <v>0</v>
       </c>
       <c r="N15" s="75">
         <f>Model!E19</f>
-        <v>-1068.2044630355258</v>
+        <v>0</v>
       </c>
       <c r="O15" s="75">
         <f>Model!F19</f>
-        <v>-1097.2733122184582</v>
+        <v>0</v>
       </c>
       <c r="P15" s="75">
         <f>Model!G19</f>
-        <v>-1127.1332065824029</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="75">
         <f>Model!H19</f>
-        <v>-1157.8056726926004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="75" x14ac:dyDescent="0.25">
@@ -2578,23 +2578,23 @@
       <c r="L16" s="15"/>
       <c r="M16" s="75">
         <f>Model!D22</f>
-        <v>-576.1076583314034</v>
+        <v>0</v>
       </c>
       <c r="N16" s="75">
         <f>Model!E22</f>
-        <v>-17.896209292237543</v>
+        <v>0</v>
       </c>
       <c r="O16" s="75">
         <f>Model!F22</f>
-        <v>-16.164516662814123</v>
+        <v>0</v>
       </c>
       <c r="P16" s="75">
         <f>Model!G22</f>
-        <v>-16.60439864538052</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="75">
         <f>Model!H22</f>
-        <v>-17.056251054444832</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="75" x14ac:dyDescent="0.25">
@@ -2624,23 +2624,23 @@
       <c r="L17" s="15"/>
       <c r="M17" s="75">
         <f>Model!D23</f>
-        <v>-354.13365014804413</v>
+        <v>0</v>
       </c>
       <c r="N17" s="75">
         <f>Model!E23</f>
-        <v>-11.000808319107122</v>
+        <v>0</v>
       </c>
       <c r="O17" s="75">
         <f>Model!F23</f>
-        <v>-9.9363360404910814</v>
+        <v>0</v>
       </c>
       <c r="P17" s="75">
         <f>Model!G23</f>
-        <v>-10.206731703294416</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="75">
         <f>Model!H23</f>
-        <v>-10.484485592929543</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="75" x14ac:dyDescent="0.25">
@@ -2670,23 +2670,23 @@
       <c r="L18" s="15"/>
       <c r="M18" s="75">
         <f>Model!D24</f>
-        <v>-105.78018121305216</v>
+        <v>0</v>
       </c>
       <c r="N18" s="75">
         <f>Model!E24</f>
-        <v>-3.2859557316813484</v>
+        <v>0</v>
       </c>
       <c r="O18" s="75">
         <f>Model!F24</f>
-        <v>-2.9679964796272067</v>
+        <v>0</v>
       </c>
       <c r="P18" s="75">
         <f>Model!G24</f>
-        <v>-3.0487640152697613</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="75">
         <f>Model!H24</f>
-        <v>-3.1317294628231109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="75" x14ac:dyDescent="0.25">
@@ -2808,23 +2808,23 @@
       <c r="L21" s="15"/>
       <c r="M21" s="75">
         <f>Model!D27</f>
-        <v>-576.1076583314034</v>
+        <v>0</v>
       </c>
       <c r="N21" s="75">
         <f>Model!E27</f>
-        <v>-594.00386762364099</v>
+        <v>0</v>
       </c>
       <c r="O21" s="75">
         <f>Model!F27</f>
-        <v>-610.16838428645508</v>
+        <v>0</v>
       </c>
       <c r="P21" s="75">
         <f>Model!G27</f>
-        <v>-626.77278293183565</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="75">
         <f>Model!H27</f>
-        <v>-643.82903398628048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="75" x14ac:dyDescent="0.25">
@@ -2854,23 +2854,23 @@
       <c r="L22" s="15"/>
       <c r="M22" s="75">
         <f>Model!D28</f>
-        <v>-354.13365014804413</v>
+        <v>0</v>
       </c>
       <c r="N22" s="75">
         <f>Model!E28</f>
-        <v>-365.13445846715126</v>
+        <v>0</v>
       </c>
       <c r="O22" s="75">
         <f>Model!F28</f>
-        <v>-375.07079450764235</v>
+        <v>0</v>
       </c>
       <c r="P22" s="75">
         <f>Model!G28</f>
-        <v>-385.27752621093674</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="75">
         <f>Model!H28</f>
-        <v>-395.7620118038663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="75" x14ac:dyDescent="0.25">
@@ -2900,23 +2900,23 @@
       <c r="L23" s="15"/>
       <c r="M23" s="75">
         <f>Model!D29</f>
-        <v>-105.78018121305216</v>
+        <v>0</v>
       </c>
       <c r="N23" s="75">
         <f>Model!E29</f>
-        <v>-109.06613694473351</v>
+        <v>0</v>
       </c>
       <c r="O23" s="75">
         <f>Model!F29</f>
-        <v>-112.03413342436072</v>
+        <v>0</v>
       </c>
       <c r="P23" s="75">
         <f>Model!G29</f>
-        <v>-115.08289743963047</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="75">
         <f>Model!H29</f>
-        <v>-118.21462690245359</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="75" x14ac:dyDescent="0.25">
@@ -2948,23 +2948,23 @@
       </c>
       <c r="M24" s="75">
         <f>Model!D30</f>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
       <c r="N24" s="75">
         <f>Model!E30</f>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
       <c r="O24" s="75">
         <f>Model!F30</f>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
       <c r="P24" s="75">
         <f>Model!G30</f>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="75">
         <f>Model!H30</f>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="75" x14ac:dyDescent="0.25">
@@ -2996,23 +2996,23 @@
       </c>
       <c r="M25" s="75">
         <f>Model!D31</f>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
       <c r="N25" s="75">
         <f>Model!E31</f>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
       <c r="O25" s="75">
         <f>Model!F31</f>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
       <c r="P25" s="75">
         <f>Model!G31</f>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="75">
         <f>Model!H31</f>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="75" x14ac:dyDescent="0.25">
@@ -3044,23 +3044,23 @@
       </c>
       <c r="M26" s="75">
         <f>Model!D32</f>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
       <c r="N26" s="75">
         <f>Model!E32</f>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
       <c r="O26" s="75">
         <f>Model!F32</f>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
       <c r="P26" s="75">
         <f>Model!G32</f>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="75">
         <f>Model!H32</f>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -3306,7 +3306,7 @@
       <c r="L33" s="15"/>
       <c r="N33" s="24">
         <f>Model!E42</f>
-        <v>2.93</v>
+        <v>3.4672898500000002</v>
       </c>
       <c r="O33" s="24">
         <f>Model!F42</f>
@@ -3631,7 +3631,7 @@
       </c>
       <c r="C4" s="4">
         <f>machine_readable!M2</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4">
         <f>machine_readable!N2</f>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D5" s="4">
         <f>machine_readable!N3</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4">
         <f>machine_readable!O3</f>
@@ -3687,11 +3687,11 @@
       </c>
       <c r="C6" s="68">
         <f t="shared" ref="C6:G6" si="2">C4-C5</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D6" s="68">
         <f t="shared" si="2"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="E6" s="68">
         <f t="shared" si="2"/>
@@ -3726,23 +3726,23 @@
       </c>
       <c r="C10" s="13">
         <f>Model!D53</f>
-        <v>36.021489692499657</v>
+        <v>0</v>
       </c>
       <c r="D10" s="13">
         <f>Model!E53</f>
-        <v>37.182973343026013</v>
+        <v>0</v>
       </c>
       <c r="E10" s="13">
         <f>Model!F53</f>
-        <v>29.068849182932411</v>
+        <v>0</v>
       </c>
       <c r="F10" s="13">
         <f>Model!G53</f>
-        <v>29.859894363944697</v>
+        <v>0</v>
       </c>
       <c r="G10" s="13">
         <f>Model!H53</f>
-        <v>30.672466110197487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3754,23 +3754,23 @@
       </c>
       <c r="C11" s="13">
         <f>Model!D54</f>
-        <v>1036.0214896924997</v>
+        <v>0</v>
       </c>
       <c r="D11" s="13">
         <f>Model!E54</f>
-        <v>1068.2044630355258</v>
+        <v>0</v>
       </c>
       <c r="E11" s="13">
         <f>Model!F54</f>
-        <v>1097.2733122184582</v>
+        <v>0</v>
       </c>
       <c r="F11" s="13">
         <f>Model!G54</f>
-        <v>1127.1332065824029</v>
+        <v>0</v>
       </c>
       <c r="G11" s="13">
         <f>Model!H54</f>
-        <v>1157.8056726926004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3782,23 +3782,23 @@
       </c>
       <c r="C12" s="13">
         <f>Model!D53+Model!D6</f>
-        <v>1036.0214896924997</v>
+        <v>0</v>
       </c>
       <c r="D12" s="13">
         <f>Model!E53+Model!E6</f>
-        <v>32.182973343026013</v>
+        <v>0</v>
       </c>
       <c r="E12" s="13">
         <f>Model!F53+Model!F6</f>
-        <v>29.068849182932411</v>
+        <v>0</v>
       </c>
       <c r="F12" s="13">
         <f>Model!G53+Model!G6</f>
-        <v>29.859894363944697</v>
+        <v>0</v>
       </c>
       <c r="G12" s="13">
         <f>Model!H53+Model!H6</f>
-        <v>30.672466110197487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3810,23 +3810,23 @@
       </c>
       <c r="C13" s="51">
         <f>SUM($C10:C10)</f>
-        <v>36.021489692499657</v>
+        <v>0</v>
       </c>
       <c r="D13" s="51">
         <f>SUM($C10:D10)</f>
-        <v>73.204463035525663</v>
+        <v>0</v>
       </c>
       <c r="E13" s="51">
         <f>SUM($C10:E10)</f>
-        <v>102.27331221845807</v>
+        <v>0</v>
       </c>
       <c r="F13" s="51">
         <f>SUM($C10:F10)</f>
-        <v>132.13320658240278</v>
+        <v>0</v>
       </c>
       <c r="G13" s="51">
         <f>SUM($C10:G10)</f>
-        <v>162.80567269260027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="D4" s="4">
         <f>'For user (EN)'!C4</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="4">
         <f>'For user (EN)'!D4</f>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="E5" s="68">
         <f>'For user (EN)'!D5</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F5" s="68">
         <f>'For user (EN)'!E5</f>
@@ -3996,11 +3996,11 @@
       </c>
       <c r="D6" s="68">
         <f>'For user (EN)'!C6</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E6" s="68">
         <f>'For user (EN)'!D6</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F6" s="68">
         <f>'For user (EN)'!E6</f>
@@ -4187,11 +4187,11 @@
       <c r="C16" s="30"/>
       <c r="D16" s="9">
         <f>(D13/100)*D6</f>
-        <v>36.021489692499657</v>
+        <v>0</v>
       </c>
       <c r="E16" s="9">
         <f>(E13/100)*E6</f>
-        <v>-0.13606406914050523</v>
+        <v>0</v>
       </c>
       <c r="F16" s="9">
         <f t="shared" ref="F16:H16" si="1">(F13/100)*F6</f>
@@ -4220,19 +4220,19 @@
       </c>
       <c r="E17" s="9">
         <f>(D50/100)*D54</f>
-        <v>37.319037412166516</v>
+        <v>0</v>
       </c>
       <c r="F17" s="9">
         <f>(E50/100)*E54</f>
-        <v>29.068849182932411</v>
+        <v>0</v>
       </c>
       <c r="G17" s="9">
         <f>(F50/100)*F54</f>
-        <v>29.859894363944697</v>
+        <v>0</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" ref="H17" si="2">(G50/100)*G54</f>
-        <v>30.672466110197487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -4245,23 +4245,23 @@
       <c r="C18" s="30"/>
       <c r="D18" s="9">
         <f>-(D6+D16+D17)</f>
-        <v>-1036.0214896924997</v>
+        <v>0</v>
       </c>
       <c r="E18" s="9">
         <f>-(E6+E16+E17)</f>
-        <v>-32.182973343026013</v>
+        <v>0</v>
       </c>
       <c r="F18" s="9">
         <f>-(F6+F16+F17)</f>
-        <v>-29.068849182932411</v>
+        <v>0</v>
       </c>
       <c r="G18" s="9">
         <f>-(G6+G16+G17)</f>
-        <v>-29.859894363944697</v>
+        <v>0</v>
       </c>
       <c r="H18" s="9">
         <f t="shared" ref="H18" si="3">-(H6+H16+H17)</f>
-        <v>-30.672466110197487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -4274,23 +4274,23 @@
       <c r="C19" s="30"/>
       <c r="D19" s="9">
         <f>SUM($D18:D18)</f>
-        <v>-1036.0214896924997</v>
+        <v>0</v>
       </c>
       <c r="E19" s="9">
         <f>SUM($D18:E18)</f>
-        <v>-1068.2044630355258</v>
+        <v>0</v>
       </c>
       <c r="F19" s="9">
         <f>SUM($D18:F18)</f>
-        <v>-1097.2733122184582</v>
+        <v>0</v>
       </c>
       <c r="G19" s="9">
         <f>SUM($D18:G18)</f>
-        <v>-1127.1332065824029</v>
+        <v>0</v>
       </c>
       <c r="H19" s="9">
         <f>SUM($D18:H18)</f>
-        <v>-1157.8056726926004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -4325,23 +4325,23 @@
       <c r="C22" s="30"/>
       <c r="D22" s="9">
         <f>SUM(D18,D35,D39)*'Fiscal Model Import'!E2</f>
-        <v>-576.1076583314034</v>
+        <v>0</v>
       </c>
       <c r="E22" s="9">
         <f>SUM(E18,E35,E39)*'Fiscal Model Import'!F2</f>
-        <v>-17.896209292237543</v>
+        <v>0</v>
       </c>
       <c r="F22" s="9">
         <f>SUM(F18,F35,F39)*'Fiscal Model Import'!G2</f>
-        <v>-16.164516662814123</v>
+        <v>0</v>
       </c>
       <c r="G22" s="9">
         <f>SUM(G18,G35,G39)*'Fiscal Model Import'!H2</f>
-        <v>-16.60439864538052</v>
+        <v>0</v>
       </c>
       <c r="H22" s="9">
         <f>SUM(H18,H35,H39)*'Fiscal Model Import'!I2</f>
-        <v>-17.056251054444832</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -4354,23 +4354,23 @@
       <c r="C23" s="30"/>
       <c r="D23" s="69">
         <f>SUM(D18,D35,D39)*'Fiscal Model Import'!E4</f>
-        <v>-354.13365014804413</v>
+        <v>0</v>
       </c>
       <c r="E23" s="69">
         <f>SUM(E18,E35,E39)*'Fiscal Model Import'!F4</f>
-        <v>-11.000808319107122</v>
+        <v>0</v>
       </c>
       <c r="F23" s="69">
         <f>SUM(F18,F35,F39)*'Fiscal Model Import'!G4</f>
-        <v>-9.9363360404910814</v>
+        <v>0</v>
       </c>
       <c r="G23" s="69">
         <f>SUM(G18,G35,G39)*'Fiscal Model Import'!H4</f>
-        <v>-10.206731703294416</v>
+        <v>0</v>
       </c>
       <c r="H23" s="69">
         <f>SUM(H18,H35,H39)*'Fiscal Model Import'!I4</f>
-        <v>-10.484485592929543</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -4383,23 +4383,23 @@
       <c r="C24" s="30"/>
       <c r="D24" s="69">
         <f>SUM(D18,D35,D39)*'Fiscal Model Import'!E3</f>
-        <v>-105.78018121305216</v>
+        <v>0</v>
       </c>
       <c r="E24" s="69">
         <f>SUM(E18,E35,E39)*'Fiscal Model Import'!F3</f>
-        <v>-3.2859557316813484</v>
+        <v>0</v>
       </c>
       <c r="F24" s="69">
         <f>SUM(F18,F35,F39)*'Fiscal Model Import'!G3</f>
-        <v>-2.9679964796272067</v>
+        <v>0</v>
       </c>
       <c r="G24" s="69">
         <f>SUM(G18,G35,G39)*'Fiscal Model Import'!H3</f>
-        <v>-3.0487640152697613</v>
+        <v>0</v>
       </c>
       <c r="H24" s="69">
         <f>SUM(H18,H35,H39)*'Fiscal Model Import'!I3</f>
-        <v>-3.1317294628231109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4470,23 +4470,23 @@
       <c r="C27" s="30"/>
       <c r="D27" s="9">
         <f>D22</f>
-        <v>-576.1076583314034</v>
+        <v>0</v>
       </c>
       <c r="E27" s="69">
         <f>IF(AND(SUM(E$18,E$35,E$39)&gt;0,E19&gt;0),D27+E22-E35,E$19*D30)</f>
-        <v>-594.00386762364099</v>
+        <v>0</v>
       </c>
       <c r="F27" s="69">
         <f>IF(AND(SUM(F$18,F$35,F$39)&gt;0,F19&gt;0),E27+F22-F35,F$19*E30)</f>
-        <v>-610.16838428645508</v>
+        <v>0</v>
       </c>
       <c r="G27" s="69">
         <f t="shared" ref="G27:H27" si="4">IF(AND(SUM(G$18,G$35,G$39)&gt;0,G19&gt;0),F27+G22-G35,G$19*F30)</f>
-        <v>-626.77278293183565</v>
+        <v>0</v>
       </c>
       <c r="H27" s="69">
         <f t="shared" si="4"/>
-        <v>-643.82903398628048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -4499,23 +4499,23 @@
       <c r="C28" s="30"/>
       <c r="D28" s="69">
         <f>D23</f>
-        <v>-354.13365014804413</v>
+        <v>0</v>
       </c>
       <c r="E28" s="69">
         <f>IF(AND(SUM(E$18,E$35,E$39)&gt;0,E19&gt;0),D28+E23-E39,E$19*D31)</f>
-        <v>-365.13445846715126</v>
+        <v>0</v>
       </c>
       <c r="F28" s="69">
         <f t="shared" ref="F28:H28" si="5">IF(AND(SUM(F$18,F$35,F$39)&gt;0,F19&gt;0),E28+F23-F39,F$19*E31)</f>
-        <v>-375.07079450764235</v>
+        <v>0</v>
       </c>
       <c r="G28" s="69">
         <f t="shared" si="5"/>
-        <v>-385.27752621093674</v>
+        <v>0</v>
       </c>
       <c r="H28" s="69">
         <f t="shared" si="5"/>
-        <v>-395.7620118038663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
@@ -4528,23 +4528,23 @@
       <c r="C29" s="30"/>
       <c r="D29" s="69">
         <f>D24</f>
-        <v>-105.78018121305216</v>
+        <v>0</v>
       </c>
       <c r="E29" s="69">
         <f>IF(AND(SUM(E$18,E$35,E$39)&gt;0,E19&gt;0),D29+E24,E$19*D32)</f>
-        <v>-109.06613694473351</v>
+        <v>0</v>
       </c>
       <c r="F29" s="69">
         <f t="shared" ref="F29:H29" si="6">IF(AND(SUM(F$18,F$35,F$39)&gt;0,F19&gt;0),E29+F24,F$19*E32)</f>
-        <v>-112.03413342436072</v>
+        <v>0</v>
       </c>
       <c r="G29" s="69">
         <f t="shared" si="6"/>
-        <v>-115.08289743963047</v>
+        <v>0</v>
       </c>
       <c r="H29" s="69">
         <f t="shared" si="6"/>
-        <v>-118.21462690245359</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -4557,23 +4557,23 @@
       <c r="C30" s="30"/>
       <c r="D30" s="67">
         <f>IF(D19=0,0,D27/D19)</f>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
       <c r="E30" s="67">
         <f t="shared" ref="E30:H30" si="7">IF(E19=0,0,E27/E19)</f>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
       <c r="F30" s="67">
         <f>IF(F19=0,0,F27/F19)</f>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
       <c r="G30" s="67">
         <f t="shared" si="7"/>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
       <c r="H30" s="67">
         <f t="shared" si="7"/>
-        <v>0.55607693861871266</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4586,23 +4586,23 @@
       <c r="C31" s="30"/>
       <c r="D31" s="67">
         <f>IF(D19=0,0,D28/D19)</f>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
       <c r="E31" s="67">
         <f t="shared" ref="E31:H31" si="8">IF(E19=0,0,E28/E19)</f>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
       <c r="F31" s="67">
         <f t="shared" si="8"/>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
       <c r="G31" s="67">
         <f t="shared" si="8"/>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
       <c r="H31" s="67">
         <f t="shared" si="8"/>
-        <v>0.34182075726359124</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -4615,23 +4615,23 @@
       <c r="C32" s="30"/>
       <c r="D32" s="67">
         <f>IF(D19=0,0,D29/D19)</f>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
       <c r="E32" s="67">
         <f t="shared" ref="E32:H32" si="9">IF(E19=0,0,E29/E19)</f>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
       <c r="F32" s="67">
         <f t="shared" si="9"/>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
       <c r="G32" s="67">
         <f t="shared" si="9"/>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
       <c r="H32" s="67">
         <f t="shared" si="9"/>
-        <v>0.10210230411769609</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -4808,7 +4808,7 @@
       <c r="D42" s="46"/>
       <c r="E42" s="32">
         <f>IF(D19&lt;0,E12,D12)</f>
-        <v>2.93</v>
+        <v>3.4672898500000002</v>
       </c>
       <c r="F42" s="32">
         <f>IF(OR(E19&lt;0,(E28-F39)=0),F12,(E47*E28-F41*F39)/(E28-F39))</f>
@@ -5023,23 +5023,23 @@
       <c r="C53" s="12"/>
       <c r="D53" s="13">
         <f>D16+D17</f>
-        <v>36.021489692499657</v>
+        <v>0</v>
       </c>
       <c r="E53" s="13">
         <f>E16+E17</f>
-        <v>37.182973343026013</v>
+        <v>0</v>
       </c>
       <c r="F53" s="13">
         <f>F16+F17</f>
-        <v>29.068849182932411</v>
+        <v>0</v>
       </c>
       <c r="G53" s="13">
         <f t="shared" ref="G53:H53" si="18">G16+G17</f>
-        <v>29.859894363944697</v>
+        <v>0</v>
       </c>
       <c r="H53" s="13">
         <f t="shared" si="18"/>
-        <v>30.672466110197487</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -5050,23 +5050,23 @@
       <c r="C54" s="12"/>
       <c r="D54" s="13">
         <f t="shared" ref="D54:H54" si="19">-D19</f>
-        <v>1036.0214896924997</v>
+        <v>0</v>
       </c>
       <c r="E54" s="13">
         <f t="shared" si="19"/>
-        <v>1068.2044630355258</v>
+        <v>0</v>
       </c>
       <c r="F54" s="13">
         <f t="shared" si="19"/>
-        <v>1097.2733122184582</v>
+        <v>0</v>
       </c>
       <c r="G54" s="13">
         <f t="shared" si="19"/>
-        <v>1127.1332065824029</v>
+        <v>0</v>
       </c>
       <c r="H54" s="13">
         <f t="shared" si="19"/>
-        <v>1157.8056726926004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -5077,23 +5077,23 @@
       <c r="C55" s="12"/>
       <c r="D55" s="13">
         <f>SUM($D53:D53)</f>
-        <v>36.021489692499657</v>
+        <v>0</v>
       </c>
       <c r="E55" s="13">
         <f>SUM($D53:E53)</f>
-        <v>73.204463035525663</v>
+        <v>0</v>
       </c>
       <c r="F55" s="13">
         <f>SUM($D53:F53)</f>
-        <v>102.27331221845807</v>
+        <v>0</v>
       </c>
       <c r="G55" s="13">
         <f>SUM($D53:G53)</f>
-        <v>132.13320658240278</v>
+        <v>0</v>
       </c>
       <c r="H55" s="13">
         <f>SUM($D53:H53)</f>
-        <v>162.80567269260027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Replaced payload file with missing label.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hoc-cdc.ca\AdminPrivate\FS06U\VanheR\Downloads\WORKDIR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\WORKDIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E9E4E5C-2E67-4DD4-B094-C8CD722F4D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FD6E6A1-B2F0-4B51-AB3D-787E2CFAA9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
   </bookViews>
   <sheets>
     <sheet name="How to interface with Web tool" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="270">
   <si>
     <t>INPUTS</t>
   </si>
@@ -846,6 +846,9 @@
   </si>
   <si>
     <t>Encours des obligations à long terme</t>
+  </si>
+  <si>
+    <t>Surplus/(deficit) for the year</t>
   </si>
 </sst>
 </file>
@@ -1779,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DA5658-E2EA-4E0B-B547-2D4F388F10E4}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C1:C19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,7 +2028,7 @@
         <v>215</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>220</v>
+        <v>269</v>
       </c>
       <c r="D6" s="73" t="s">
         <v>220</v>
@@ -2680,8 +2683,8 @@
   </sheetPr>
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3951,8 +3954,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>